<commit_message>
updated OSILong with corrected values (since OXY changed). re-ran stats in OSI scripts, pretty much exactly the same
</commit_message>
<xml_diff>
--- a/GreenIguanaMasterSpring2021_OXYredo.xlsx
+++ b/GreenIguanaMasterSpring2021_OXYredo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\OneDrive - USU\Desktop\ASU green iguana 2021\greeniguanaAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E8217D-6601-4E04-94C6-6803D7AE7805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FE9123-A790-44F6-BBFC-9699632E17D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="270" windowWidth="25440" windowHeight="15270" xr2:uid="{05DEEAC3-4815-49FC-A89C-2E5FF095514B}"/>
   </bookViews>
@@ -1069,7 +1069,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1080,8 +1080,8 @@
   <dimension ref="A1:GP37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="FG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="FQ22" sqref="FQ22"/>
+      <pane xSplit="1" topLeftCell="FN1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="FX1" sqref="FX1:GJ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2772,11 +2772,11 @@
         <v>-1.7017608034624829</v>
       </c>
       <c r="FZ3">
-        <f t="shared" ref="FZ3:FZ37" si="2">EZ3-FM3</f>
+        <f t="shared" ref="FZ3:FZ36" si="2">EZ3-FM3</f>
         <v>0.98272503532309763</v>
       </c>
       <c r="GA3">
-        <f t="shared" ref="GA3:GA37" si="3">FA3-FN3</f>
+        <f t="shared" ref="GA3:GA36" si="3">FA3-FN3</f>
         <v>-2.9574363703750617</v>
       </c>
       <c r="GB3">

</xml_diff>